<commit_message>
Adjusted column widths and formatted cells for better visualisation. Protected all the cells except the ones that users put their grades.
</commit_message>
<xml_diff>
--- a/sample_grades.xlsx
+++ b/sample_grades.xlsx
@@ -1,15 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egeal\PycharmProjects\IEU-Grade-Calculator-Excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6207CF7-72A0-480A-881D-3AD529E2BF96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Courses" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -67,9 +85,17 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -97,14 +123,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -151,7 +189,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -183,9 +221,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -217,6 +273,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -392,28 +466,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="2" max="3" width="7.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -423,8 +503,11 @@
       <c r="C2">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="D2" s="2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -434,8 +517,12 @@
       <c r="C3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="D3" s="2">
+        <f>AVERAGE(50,50,50,100)</f>
+        <v>62.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -445,8 +532,11 @@
       <c r="C4">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="D4" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -456,28 +546,31 @@
       <c r="C5">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="D5" s="2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D6">
         <f>SUMPRODUCT(C2:C5,D2:D5)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
+        <v>83.850000000000009</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -487,8 +580,11 @@
       <c r="C8">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="D8" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -498,8 +594,11 @@
       <c r="C9">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="D9" s="2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -509,28 +608,31 @@
       <c r="C10">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="D10" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D11">
         <f>SUMPRODUCT(C8:C10,D8:D10)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
+        <v>64.400000000000006</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -540,8 +642,12 @@
       <c r="C13">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="D13" s="2">
+        <f>800/9</f>
+        <v>88.888888888888886</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -551,8 +657,12 @@
       <c r="C14">
         <v>0.08</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="D14" s="2">
+        <f>AVERAGE(100,30,50,50)</f>
+        <v>57.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -562,8 +672,11 @@
       <c r="C15">
         <v>0.26</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="D15" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -573,28 +686,31 @@
       <c r="C16">
         <v>0.42</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="D16" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D17">
         <f>SUMPRODUCT(C13:C16,D13:D16)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
+        <v>93.933333333333337</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -604,8 +720,11 @@
       <c r="C19">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="D19" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -615,8 +734,11 @@
       <c r="C20">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="D20" s="2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -626,8 +748,12 @@
       <c r="C21">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="D21" s="2">
+        <f>AVERAGE(85, 71)</f>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -637,28 +763,31 @@
       <c r="C22">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="D22" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D23">
         <f>SUMPRODUCT(C19:C22,D19:D22)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" t="s">
+        <v>61.7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -668,8 +797,11 @@
       <c r="C25">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="D25" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -679,8 +811,11 @@
       <c r="C26">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="D26" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>2</v>
       </c>
@@ -690,8 +825,11 @@
       <c r="C27">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="D27" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -701,8 +839,11 @@
       <c r="C28">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="D28" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>3</v>
       </c>
@@ -712,8 +853,11 @@
       <c r="C29">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="D29" s="2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -723,14 +867,18 @@
       <c r="C30">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="D30" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D31">
         <f>SUMPRODUCT(C25:C30,D25:D30)</f>
-        <v>0</v>
+        <v>94.8</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>